<commit_message>
task planning so not lost in pc reset
</commit_message>
<xml_diff>
--- a/TFE/Development/Planning/TaskPlanning.xlsx
+++ b/TFE/Development/Planning/TaskPlanning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21651B69-FA08-4D49-82D8-E64C6B0D4E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E369DC-6AEA-4F63-B758-FC3568E1154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="300">
   <si>
     <t>Task</t>
   </si>
@@ -937,6 +937,12 @@
   </si>
   <si>
     <t>This is pretty much EG though….</t>
+  </si>
+  <si>
+    <t>Package the Objective Points mod stuff into the main mod</t>
+  </si>
+  <si>
+    <t>Flayed ones are immortal when coming out of the ground, how to change this?</t>
   </si>
 </sst>
 </file>
@@ -3313,13 +3319,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE0C65C-144B-49AC-9C67-3120B47D1850}">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F118" sqref="F118"/>
+      <selection pane="bottomRight" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,6 +5450,23 @@
         <v>21</v>
       </c>
       <c r="E118" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="B119" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5825,10 +5848,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6383,7 +6406,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G30" s="56" t="s">
         <v>279</v>
@@ -8571,7 +8594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB2C39-26AB-4D6A-97C6-B18CDA37BA1E}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9913,7 +9936,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9953,6 +9976,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[ELDAR] Remove depreciated farseer variants
</commit_message>
<xml_diff>
--- a/TFE/Development/Planning/TaskPlanning.xlsx
+++ b/TFE/Development/Planning/TaskPlanning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E369DC-6AEA-4F63-B758-FC3568E1154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A970A75E-C4E6-46B4-A4F5-180FE6C78A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="9" r:id="rId1"/>
@@ -3322,10 +3322,10 @@
   <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E119" sqref="E119"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,7 +4047,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>